<commit_message>
feat: HUD UI 增加小地图
</commit_message>
<xml_diff>
--- a/Config/Habitats.xlsx
+++ b/Config/Habitats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\university\graduation-design\habitats-exploration\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA42A50A-F81C-4AEF-91E6-337532120761}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E86C19-391D-4377-96B4-B5D09DD9C6FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1095" yWindow="-120" windowWidth="27825" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -93,6 +93,14 @@
   </si>
   <si>
     <t>沼泽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Minimap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小地图</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -439,23 +447,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C319EAB0-E15C-48AE-9953-B84954D6139C}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9" style="3"/>
-    <col min="2" max="2" width="13" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10.625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="4"/>
+    <col min="1" max="1" width="12.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="4" customWidth="1"/>
+    <col min="3" max="3" width="20.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.5" style="4" customWidth="1"/>
+    <col min="6" max="6" width="29.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -471,8 +479,11 @@
       <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -488,8 +499,11 @@
       <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -505,8 +519,11 @@
       <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -523,8 +540,12 @@
       <c r="E4" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="3" t="str">
+        <f>CONCATENATE("tex_habitats_minimap_",B4,".png")</f>
+        <v>tex_habitats_minimap_山谷.png</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -541,8 +562,12 @@
       <c r="E5" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="3" t="str">
+        <f t="shared" ref="F5:F6" si="1">CONCATENATE("tex_habitats_minimap_",B5,".png")</f>
+        <v>tex_habitats_minimap_密林.png</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -559,44 +584,48 @@
       <c r="E6" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>tex_habitats_minimap_沼泽.png</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
     </row>

</xml_diff>